<commit_message>
Added extra figures and updated the BOM for V3.1.
</commit_message>
<xml_diff>
--- a/Hardware/BOM BLE BoosterPack V3_1.xlsx
+++ b/Hardware/BOM BLE BoosterPack V3_1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Description</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>1uF</t>
-  </si>
-  <si>
     <t>0.001uF</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
   </si>
   <si>
     <t>10k</t>
-  </si>
-  <si>
-    <t>1k</t>
   </si>
   <si>
     <t>2k</t>
@@ -567,7 +561,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="6"/>
@@ -611,10 +605,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3"/>
       <c r="F3" s="8"/>
@@ -624,10 +618,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3"/>
       <c r="F4" s="8"/>
@@ -637,10 +631,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5" s="3"/>
       <c r="F5" s="8"/>
@@ -650,10 +644,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6" s="3"/>
       <c r="F6" s="8"/>
@@ -663,10 +657,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="D7" s="3"/>
       <c r="F7" s="8"/>
@@ -676,10 +670,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3"/>
       <c r="F8" s="8"/>
@@ -689,10 +683,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3"/>
       <c r="F9" s="8"/>
@@ -702,10 +696,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
         <v>54</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
       </c>
       <c r="D10" s="3"/>
       <c r="F10" s="8"/>
@@ -715,10 +709,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3"/>
       <c r="F11" s="8"/>
@@ -728,10 +722,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D12" s="3"/>
       <c r="F12" s="8"/>
@@ -741,10 +735,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
       </c>
       <c r="D13" s="3"/>
       <c r="F13" s="8"/>
@@ -754,10 +751,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
       </c>
       <c r="D14" s="3"/>
       <c r="F14" s="8"/>
@@ -767,13 +767,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" s="3"/>
       <c r="F15" s="8"/>
@@ -783,13 +783,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="D16" s="3"/>
       <c r="F16" s="8"/>
@@ -799,10 +799,10 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
         <v>36</v>
@@ -815,13 +815,13 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" t="s">
-        <v>58</v>
+      <c r="C18" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D18" s="3"/>
       <c r="F18" s="8"/>
@@ -831,13 +831,13 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19" s="3"/>
       <c r="F19" s="8"/>
@@ -847,13 +847,13 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>39</v>
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
       </c>
       <c r="D20" s="3"/>
       <c r="F20" s="8"/>
@@ -863,13 +863,13 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
         <v>12</v>
       </c>
-      <c r="B21" t="s">
-        <v>31</v>
-      </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D21" s="3"/>
       <c r="F21" s="8"/>
@@ -879,13 +879,13 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D22" s="3"/>
       <c r="F22" s="8"/>
@@ -895,13 +895,13 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D23" s="3"/>
       <c r="F23" s="8"/>
@@ -911,13 +911,13 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D24" s="3"/>
       <c r="F24" s="8"/>
@@ -927,13 +927,13 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D25" s="3"/>
       <c r="F25" s="8"/>
@@ -946,10 +946,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="D26" s="3"/>
       <c r="F26" s="8"/>
@@ -959,13 +959,13 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D27" s="3"/>
       <c r="F27" s="8"/>
@@ -975,13 +975,13 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D28" s="3"/>
       <c r="F28" s="8"/>
@@ -990,15 +990,6 @@
       <c r="L28" s="8"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" t="s">
-        <v>32</v>
-      </c>
       <c r="D29" s="3"/>
       <c r="F29" s="8"/>
       <c r="H29" s="8"/>
@@ -1006,15 +997,6 @@
       <c r="L29" s="8"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" t="s">
-        <v>46</v>
-      </c>
       <c r="D30" s="3"/>
       <c r="F30" s="8"/>
       <c r="H30" s="8"/>

</xml_diff>